<commit_message>
inserimento id e nome
</commit_message>
<xml_diff>
--- a/Informatica/GruppoOilPrototipo/bin/Debug/Misurazioni/template.xlsx
+++ b/Informatica/GruppoOilPrototipo/bin/Debug/Misurazioni/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolas\OneDrive\Desktop\Gruppo-Oil_progetto-Omb-Vales\Informatica\GruppoOilPrototipo\bin\Debug\Misurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBD73A64-5144-40FC-AF05-2016BF87073A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6326D8F7-3303-4EA5-A7ED-0AF4B236C6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D22987AD-16C1-4A34-B077-E291DE592DA1}"/>
   </bookViews>
@@ -99,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -107,7 +107,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -192,7 +191,7 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:numRef>
+                  <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -200,7 +199,7 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:numRef>
+                  </c:multiLvlStrRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -1267,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0138E0E6-48A8-41FC-B44B-6002F3B33E3F}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,7 +1279,7 @@
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1289,75 +1288,76 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Revert "inserimento id e nome"
This reverts commit 43b0c51b226189778350b476579aa4300a74b61e.
</commit_message>
<xml_diff>
--- a/Informatica/GruppoOilPrototipo/bin/Debug/Misurazioni/template.xlsx
+++ b/Informatica/GruppoOilPrototipo/bin/Debug/Misurazioni/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolas\OneDrive\Desktop\Gruppo-Oil_progetto-Omb-Vales\Informatica\GruppoOilPrototipo\bin\Debug\Misurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6326D8F7-3303-4EA5-A7ED-0AF4B236C6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBD73A64-5144-40FC-AF05-2016BF87073A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D22987AD-16C1-4A34-B077-E291DE592DA1}"/>
   </bookViews>
@@ -99,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -107,6 +107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -191,7 +192,7 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:multiLvlStrRef>
+                  <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -199,7 +200,7 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:multiLvlStrRef>
+                  </c:numRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -1266,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0138E0E6-48A8-41FC-B44B-6002F3B33E3F}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1279,7 +1280,7 @@
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1288,76 +1289,75 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>